<commit_message>
NB Reporting: 1) added NICK MF expenses for correct calculation of capital (kzt form 6) 2) kzt form 19 - export template cell formatting
</commit_message>
<xml_diff>
--- a/nicnbk-data/nicnbk-data-service-impl/src/main/resources/export_template/reporting/TEMPLATE_NICKMF_cons_KZT_19.xlsx
+++ b/nicnbk-data/nicnbk-data-service-impl/src/main/resources/export_template/reporting/TEMPLATE_NICKMF_cons_KZT_19.xlsx
@@ -109,7 +109,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₸_-;\-* #,##0.00\ _₸_-;_-* &quot;-&quot;??\ _₸_-;_-@_-"/>
+  </numFmts>
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,6 +172,14 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -202,10 +213,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -264,15 +276,19 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -591,7 +607,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="G15" sqref="E15:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1445,26 +1461,26 @@
       <c r="G8" s="13"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
@@ -1526,9 +1542,9 @@
       <c r="B15" s="22"/>
       <c r="C15" s="23"/>
       <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="19"/>
@@ -1540,7 +1556,7 @@
       <c r="G16" s="19"/>
     </row>
     <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="24" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="21"/>
@@ -1551,7 +1567,7 @@
       <c r="G17" s="21"/>
     </row>
     <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="24" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="21"/>
@@ -1562,7 +1578,7 @@
       <c r="G18" s="21"/>
     </row>
     <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="24" t="s">
         <v>22</v>
       </c>
       <c r="B19" s="21"/>
@@ -1573,7 +1589,7 @@
       <c r="G19" s="21"/>
     </row>
     <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="24" t="s">
         <v>23</v>
       </c>
       <c r="B20" s="21"/>

</xml_diff>